<commit_message>
Got permission to publish from ADW!
</commit_message>
<xml_diff>
--- a/dates.xlsx
+++ b/dates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellag\Pictures\MayDayMystery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellag\Documents\GitHub\maydaymystery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BE9DC1-92F9-4FB8-85A1-3CEB3514E7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273DF5DA-2094-4B74-B517-5550AB924CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="14">
   <si>
     <t>♦</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t>B23</t>
+  </si>
+  <si>
+    <t>RE-SCAN</t>
+  </si>
+  <si>
+    <t>AWAITING DUPLICATION</t>
+  </si>
+  <si>
+    <t>RE-SCAN, PAGE NUM</t>
+  </si>
+  <si>
+    <t>RRS</t>
+  </si>
+  <si>
+    <t>RRS, PAGE NUM</t>
   </si>
 </sst>
 </file>
@@ -671,7 +686,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -721,6 +736,8 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1082,7 +1099,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1190,9 @@
       <c r="G4" s="15">
         <v>24</v>
       </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
@@ -1182,7 +1201,7 @@
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="11">
+      <c r="E5" s="25">
         <v>36495</v>
       </c>
       <c r="F5" s="13" t="s">
@@ -1191,7 +1210,9 @@
       <c r="G5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="16"/>
+      <c r="H5" s="16" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -1560,7 +1581,7 @@
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="11">
+      <c r="E29" s="25">
         <v>39203</v>
       </c>
       <c r="F29" s="13" t="s">
@@ -1569,7 +1590,9 @@
       <c r="G29" s="15">
         <v>25</v>
       </c>
-      <c r="H29" s="16"/>
+      <c r="H29" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
@@ -1596,7 +1619,7 @@
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="11">
+      <c r="E31" s="25">
         <v>39540</v>
       </c>
       <c r="F31" s="13" t="s">
@@ -1605,7 +1628,9 @@
       <c r="G31" s="15">
         <v>14</v>
       </c>
-      <c r="H31" s="16"/>
+      <c r="H31" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
@@ -1616,7 +1641,7 @@
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="11">
+      <c r="E32" s="25">
         <v>39569</v>
       </c>
       <c r="F32" s="13" t="s">
@@ -1625,7 +1650,9 @@
       <c r="G32" s="15">
         <v>13</v>
       </c>
-      <c r="H32" s="16"/>
+      <c r="H32" s="16" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
@@ -1687,7 +1714,9 @@
       <c r="C36" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="13"/>
+      <c r="D36" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="E36" s="8">
         <v>40298</v>
       </c>
@@ -1755,7 +1784,9 @@
       <c r="C40" s="14">
         <v>20</v>
       </c>
-      <c r="D40" s="13"/>
+      <c r="D40" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="E40" s="8">
         <v>41030</v>
       </c>
@@ -1810,7 +1841,7 @@
       <c r="H43" s="16"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+      <c r="A44" s="26">
         <v>34090</v>
       </c>
       <c r="B44" s="13" t="s">
@@ -1819,7 +1850,9 @@
       <c r="C44" s="14">
         <v>16</v>
       </c>
-      <c r="D44" s="13"/>
+      <c r="D44" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="E44" s="8">
         <v>42125</v>
       </c>
@@ -1893,7 +1926,9 @@
       <c r="G48" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H48" s="16"/>
+      <c r="H48" s="16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="12">

</xml_diff>

<commit_message>
1993 and 2008 duplications
</commit_message>
<xml_diff>
--- a/dates.xlsx
+++ b/dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellag\Documents\GitHub\maydaymystery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273DF5DA-2094-4B74-B517-5550AB924CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6E1BF7-E831-4631-95DC-C53844D9B956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>RE-SCAN</t>
   </si>
   <si>
-    <t>AWAITING DUPLICATION</t>
-  </si>
-  <si>
     <t>RE-SCAN, PAGE NUM</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>RRS, PAGE NUM</t>
+  </si>
+  <si>
+    <t>DUP</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -737,7 +737,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1099,7 +1098,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1190,7 @@
         <v>24</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1211,7 +1210,7 @@
         <v>6</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1641,7 +1640,7 @@
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="25">
+      <c r="E32" s="11">
         <v>39569</v>
       </c>
       <c r="F32" s="13" t="s">
@@ -1651,7 +1650,7 @@
         <v>13</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1715,7 +1714,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" s="8">
         <v>40298</v>
@@ -1785,7 +1784,7 @@
         <v>20</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E40" s="8">
         <v>41030</v>
@@ -1841,8 +1840,8 @@
       <c r="H43" s="16"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="26">
-        <v>34090</v>
+      <c r="A44" s="17">
+        <v>34092</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>1</v>
@@ -1851,7 +1850,7 @@
         <v>16</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E44" s="8">
         <v>42125</v>
@@ -1927,7 +1926,7 @@
         <v>8</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Societas Rosicrusiana/Columbian League ?
</commit_message>
<xml_diff>
--- a/dates.xlsx
+++ b/dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellag\Documents\GitHub\maydaymystery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6188F1F1-9C86-42D6-A6B8-3D450634F07B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13F3DAF-9ED6-4D30-B0A2-5DF7B003027D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21600" yWindow="2445" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1263,8 +1263,8 @@
   </sheetPr>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,7 +1680,9 @@
       <c r="F22" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G22" s="14"/>
+      <c r="G22" s="14">
+        <v>10</v>
+      </c>
       <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>